<commit_message>
updated excel and filter for all 4 sheets
</commit_message>
<xml_diff>
--- a/Updated_Chartered_Secretary.xlsx
+++ b/Updated_Chartered_Secretary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mustk\Downloads\Dump\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mustk\OneDrive\Desktop\chartered_secretary_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C341F356-E1DC-414B-96EA-E532333E5D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D332BC-D1C7-44BE-9573-95E9AB6A2BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -4009,8 +4009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7080,7 +7080,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9394,7 +9396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>